<commit_message>
Import lab test types
</commit_message>
<xml_diff>
--- a/packages/lan/data/test_definitions.xlsx
+++ b/packages/lan/data/test_definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -1032,7 +1032,7 @@
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="168.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="168.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -5311,16 +5311,16 @@
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="48.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
@@ -5618,18 +5618,21 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
+      <c r="B20" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="2"/>
@@ -5734,23 +5737,10 @@
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -11932,7 +11922,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>

</xml_diff>